<commit_message>
update notification messages; fix bugs in whatsapp.py; update ui integrations
</commit_message>
<xml_diff>
--- a/docs/relatorio.xlsx
+++ b/docs/relatorio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,40 +446,65 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Phones</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Date Devolution</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Benefit</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Qtd</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>WhatsApp Phones</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Message</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Date Message Send</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Birthday</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Mother</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Benefit</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Qtd</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Father</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Spouse</t>
         </is>
@@ -488,138 +513,1008 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>426977-6</t>
+          <t>3607-6</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ADRIANO CARVALHO ORTENCIO</t>
+          <t>JACINTA NOELI GRIEBELER</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['4535421153' '' '']</t>
+          <t>['4599242824' False False]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RUA — R. NOE DE MEDEIROS - SAO JOSE DO ITAVO - SN</t>
+          <t>20/05/2021</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>14/09/1995</t>
+          <t>19/07/2021</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ROSANA ORTENCIO</t>
+          <t>CADEIRA DE RODAS - DEVOLUCAO</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CADEIRA DE RODAS</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ROSENIR CARVALHO</t>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *JACINTA NOELI GRIEBELER* tem como registro, um empréstimo de *CADEIRA DE RODAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>RUA — ARTHUR DA COSTA E SILVA - CENTRO - 1730</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>05/05/1952</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ERNA HAAS RAUBER</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>DEMETRIO RAUBER</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>GERVASIO GRIEBELER</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10382-6</t>
+          <t>11677-6</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>KAILANA RODRIGUES DA SILVA</t>
+          <t>CARLOS RIBEIRO ROSA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['4591569100' '4591569100' '']</t>
+          <t>['4535421120' '4797871755' False]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RUA — RUA PROJETADA - SAO JOSE DO ITAVO - SN</t>
+          <t>20/05/2021</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>18/11/2003</t>
+          <t>19/07/2021</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ROSELI RODRIGUES DA SILVA</t>
+          <t>MULETAS - DEVOLUCAO</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>CADEIRA DE RODAS</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['4797871755']</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>CELSO APARECIDO DA SILVA</t>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *CARLOS RIBEIRO ROSA* tem como registro, um empréstimo de *MULETAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>RUA — RUA PARAIBA - SAO JOSE DO ITAVO - 1573</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>17/09/1972</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>IGUES CORDEIRO DA ROSA</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>GERALDO RIBEIRO ROSA</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>426-6</t>
+          <t>3607-6</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>JAIR PLAUTH</t>
+          <t>JACINTA NOELI GRIEBELER</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['45998440285' '4599586379' '4591577686']</t>
+          <t>['4599242824' False False]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RUA — RUA RIO GRANDE DO SUL - SAO JOSE DO ITAVO - 1043</t>
+          <t>20/05/2021</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05/05/1979</t>
+          <t>19/07/2021</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>EVA PLAUTH</t>
+          <t>CADEIRA DE BANHO</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *JACINTA NOELI GRIEBELER* tem como registro, um empréstimo de *CADEIRA DE BANHO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>RUA — ARTHUR DA COSTA E SILVA - CENTRO - 1730</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>05/05/1952</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>ERNA HAAS RAUBER</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>DEMETRIO RAUBER</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>GERVASIO GRIEBELER</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>394152-7</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NATHIELI LETICIA RECKZIEGEL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['4599046648' '4599808073' False]</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>19/05/2021</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>18/07/2021</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>TIPOIA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['4599046648' '4599808073']</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *NATHIELI LETICIA RECKZIEGEL* tem como registro, um empréstimo de *TIPOIA* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>RUA — RUA DARCI LINHART - CARAMURU - SN</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>28/05/2004</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>SANDRA BATISTA DE FREITAS</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>CLICEU GERALDO RECKZIEGEL</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5828-6</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NEIVANIR LAUTHARTH ROSSINI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['4598417325' False False]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>19/05/2021</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>18/07/2021</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>MULETAS - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['4598417325']</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *NEIVANIR LAUTHARTH ROSSINI* tem como registro, um empréstimo de *MULETAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>RUA — 07 DE SETEMBRO - CENTRO - 1911</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>11/09/1953</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>NATALIA SILVEIRA LAUTHARTH</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>JOAO LUIZ LAUTHARTH</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1936-6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ROSANE MARIA WOLMUTH DA SILVA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['4599918514' False False]</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>18/05/2021</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>17/07/2021</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MULETAS - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['4599918514']</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *ROSANE MARIA WOLMUTH DA SILVA* tem como registro, um empréstimo de *MULETAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>AVENIDA — PARANA - JARDIM BELO HORIZONTE - 1585</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>02/12/1972</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>IRENA MARIA WALKER WOLMUTH</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>ARCOLI INACIO WOLMUTH</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>DIACIR FERREIRA DA SILVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4787-7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ERNO GULLICH</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['4599270625' '4599270625' False]</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>18/05/2021</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>17/07/2021</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>CADEIRA DE RODAS</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ANTONIO PLAUTH</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>SOELI DE FATIMA CARVALHO RIBEIRO</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['4599270625' '4599270625']</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *ERNO GULLICH* tem como registro, um empréstimo de *CADEIRA DE RODAS* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>RUA — 07 DE SETEMBRO - CENTRO - 1640</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>25/04/1954</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>ERNILDA GULLICH</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>LEOPOLDO GULLICH</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13796-6</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MAICO DJONATHAN GROTH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['4598198381' False False]</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>17/05/2021</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>16/07/2021</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MULETAS - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['4598198381']</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *MAICO DJONATHAN GROTH* tem como registro, um empréstimo de *MULETAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>RUA — 10 DE NOVEMBRO - CARAMURU - 1749</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>01/09/1994</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>LORI GROTH</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>AVENILDO GROTH</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>JUCIANE STELLA LUDWIG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>13796-6</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MAICO DJONATHAN GROTH</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['4598198381' False False]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>17/05/2021</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>16/07/2021</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BOTA ORTOPEDICA - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['4598198381']</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *MAICO DJONATHAN GROTH* tem como registro, um empréstimo de *BOTA ORTOPEDICA - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>RUA — 10 DE NOVEMBRO - CARAMURU - 1749</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>01/09/1994</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>LORI GROTH</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>AVENILDO GROTH</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>JUCIANE STELLA LUDWIG</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6436-6</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EVANI TEREZINHA CORADINI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['4591355947' False False]</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12/05/2021</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>11/07/2021</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>CADEIRA DE BANHO - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['4591355947']</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *EVANI TEREZINHA CORADINI* tem como registro, um empréstimo de *CADEIRA DE BANHO - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>AVENIDA — TIRADENTES - CENTRO - 1223</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>07/07/1942</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>HERMINIA CARNIEL CORADINI</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>LUIZ DORADINI</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>57832-8</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NATALINO DE ALMEIDA PERES</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['4591463393' '4591142613' False]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>11/05/2021</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10/07/2021</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BOTA ORTOPEDICA</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['4591463393' '4591142613']</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *NATALINO DE ALMEIDA PERES* tem como registro, um empréstimo de *BOTA ORTOPEDICA* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>RUA — BASE NAUTICA - ESQUINA GAUCHA - 179</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>06/11/1978</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>IRMA DE ALMEIDA</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>BASILIO PERES</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>DELFINA PALACIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>827-6</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MARIA ISOLINA SOARES</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['4591243247' False False]</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>07/05/2021</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>06/07/2021</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ANDADOR</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *MARIA ISOLINA SOARES* tem como registro, um empréstimo de *ANDADOR* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>RUA — INDEPENDENCIA - CENTRO - 1640</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>13/11/1952</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>ANA CLAUDIA BATISTA</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>DORIVAL SOARES</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>474-6</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DARCI SORGETZ</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['4591399573' False False]</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>05/05/2021</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>04/07/2021</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CADEIRA DE RODAS - DEVOLUCAO</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>['4591399573']</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Olá, esta é uma _mensagem automática_ de um sistema do *NASF Itaipulândia*.
+Informamos que o/a paciente *DARCI SORGETZ* tem como registro, um empréstimo de *CADEIRA DE RODAS - DEVOLUCAO* em nosso sistema.
+Solicitamos que CASO O PACIENTE NÃO ESTEJA UTILIZANDO ESTE MATERIAL, para que seja devolvido ao Posto de Saúde.
+Temos poucos materiais em estoque, estando em constante falta, seja consciente e colabore com a saúde do município.
+Caso já tenha devolvido o material, entre em contato para que seja retirado do nosso sistema.
+_Contatos:_
+E-mail: nasfitaipulandiapr@gmail.com
+Coordenadora do NASF: Camila Fernanda de Souza - (45) 99143-2728 / (45) 3559-1731</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>RUA — RUA PARAIBA - SAO JOSE DO ITAVO - 1927</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>25/12/1960</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>ELZIRA PLAUT SORGETZ</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>CLAUDINO SORGETZ</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>